<commit_message>
Expense Request Approver changes - 16 June
</commit_message>
<xml_diff>
--- a/TestData/TMTT0017339_EventExpense_VerifyTheCFExpenseRequestFunctionalityAsApprover.xlsx
+++ b/TestData/TMTT0017339_EventExpense_VerifyTheCFExpenseRequestFunctionalityAsApprover.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEB76CD-6D09-4902-8DBE-20292B0E3CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A0BC4C-0D8E-4024-B206-D616045A440F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="396" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="396" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExpenseRequest" sheetId="1" r:id="rId1"/>
@@ -527,7 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -764,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9211E4BF-D8C6-40F1-A79E-AB74298F258F}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -800,12 +800,12 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Event Expense - 23 July
</commit_message>
<xml_diff>
--- a/TestData/TMTT0017339_EventExpense_VerifyTheCFExpenseRequestFunctionalityAsApprover.xlsx
+++ b/TestData/TMTT0017339_EventExpense_VerifyTheCFExpenseRequestFunctionalityAsApprover.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A0BC4C-0D8E-4024-B206-D616045A440F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D8C52E-AB2C-4C43-8EDA-A0ABD8314BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="396" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>LOB</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>Reject</t>
-  </si>
-  <si>
-    <t>Clone</t>
   </si>
   <si>
     <t>Request More Information</t>
@@ -607,13 +604,13 @@
         <v>33</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
@@ -621,13 +618,13 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
         <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" t="s">
-        <v>50</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
@@ -672,13 +669,13 @@
         <v>34</v>
       </c>
       <c r="S2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="U2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -707,7 +704,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -748,7 +745,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -762,10 +759,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9211E4BF-D8C6-40F1-A79E-AB74298F258F}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,17 +792,12 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CF Expense Request - 8th Jan 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0017339_EventExpense_VerifyTheCFExpenseRequestFunctionalityAsApprover.xlsx
+++ b/TestData/TMTT0017339_EventExpense_VerifyTheCFExpenseRequestFunctionalityAsApprover.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D8C52E-AB2C-4C43-8EDA-A0ABD8314BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647EA18F-862A-42B7-808B-9842464E0C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="396" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="396" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExpenseRequest" sheetId="1" r:id="rId1"/>
@@ -171,13 +171,13 @@
     <t>Request is approved</t>
   </si>
   <si>
-    <t>Bingo@1234</t>
-  </si>
-  <si>
     <t>Amanda Donovan</t>
   </si>
   <si>
     <t>PFG Golf Event</t>
+  </si>
+  <si>
+    <t>Bingo@12345</t>
   </si>
 </sst>
 </file>
@@ -618,13 +618,13 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -723,7 +723,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,7 +745,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -762,7 +762,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -777,17 +777,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -797,7 +797,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
16Jan 2025 - Final
</commit_message>
<xml_diff>
--- a/TestData/TMTT0017339_EventExpense_VerifyTheCFExpenseRequestFunctionalityAsApprover.xlsx
+++ b/TestData/TMTT0017339_EventExpense_VerifyTheCFExpenseRequestFunctionalityAsApprover.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647EA18F-862A-42B7-808B-9842464E0C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E2F8AB-0C59-4827-A555-060BCE132551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="396" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="396" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExpenseRequest" sheetId="1" r:id="rId1"/>
@@ -126,9 +126,6 @@
     <t>Giselle Segura</t>
   </si>
   <si>
-    <t>gksegura@hl.com.test</t>
-  </si>
-  <si>
     <t>ApproverEditErrorMsg</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>Bingo@12345</t>
+  </si>
+  <si>
+    <t>lward@hl.com.test</t>
   </si>
 </sst>
 </file>
@@ -601,16 +601,16 @@
         <v>29</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
@@ -618,13 +618,13 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>48</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
@@ -666,16 +666,16 @@
         <v>18</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="U2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -704,7 +704,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -722,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -742,10 +742,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -761,7 +761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9211E4BF-D8C6-40F1-A79E-AB74298F258F}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -772,32 +772,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IWard cred updated - Event Expense - 22 May 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0017339_EventExpense_VerifyTheCFExpenseRequestFunctionalityAsApprover.xlsx
+++ b/TestData/TMTT0017339_EventExpense_VerifyTheCFExpenseRequestFunctionalityAsApprover.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E2F8AB-0C59-4827-A555-060BCE132551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B9B2D2-9094-44F1-B446-00D6035CF1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="396" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,10 +174,10 @@
     <t>PFG Golf Event</t>
   </si>
   <si>
-    <t>Bingo@12345</t>
-  </si>
-  <si>
     <t>lward@hl.com.test</t>
+  </si>
+  <si>
+    <t>Bingo@09876</t>
   </si>
 </sst>
 </file>
@@ -723,7 +723,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -742,10 +742,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>